<commit_message>
To describe negative login scenarios in more details
</commit_message>
<xml_diff>
--- a/Docs/ScenariosPassionFruit.xlsx
+++ b/Docs/ScenariosPassionFruit.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\SoftuniQA_Automation\GitHub TeamWork\Teamwork\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="7755"/>
   </bookViews>
@@ -90,9 +85,6 @@
   </si>
   <si>
     <t>1. Start Browser                                                                     2. Navigate to  URL http://localhost:60634/Account/Login            3. Enter user credentials                                                           4. Press button Login</t>
-  </si>
-  <si>
-    <t>Unsuccessful Login. An appropriate message is displayed</t>
   </si>
   <si>
     <t>Guest User tries to edit post</t>
@@ -201,6 +193,9 @@
   </si>
   <si>
     <t xml:space="preserve">1. Start Browser     2. Navigate to  URL  http://localhost:60634/Article/List    3. Check the user is logged     4. Click on Create button      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsuccessful Login. An appropriate message is displayed.  No email address entered, an appropriate message is displayed. No password entered, an appropriate message is displayed. Wrong email address fromat, an appropriate message is displayed. </t>
   </si>
 </sst>
 </file>
@@ -540,8 +535,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Хипервръзка" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -839,7 +834,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -849,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I942"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +937,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
@@ -984,7 +979,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -996,7 +991,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="I6" s="10"/>
     </row>
@@ -1005,17 +1000,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="10"/>
     </row>
@@ -1024,17 +1019,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="10"/>
     </row>
@@ -1043,17 +1038,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I9" s="10"/>
     </row>
@@ -1062,17 +1057,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="10"/>
     </row>
@@ -1081,17 +1076,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I11" s="10"/>
     </row>
@@ -1100,17 +1095,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I12" s="10"/>
     </row>
@@ -1119,17 +1114,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="10"/>
     </row>
@@ -1138,17 +1133,17 @@
         <v>13</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="37"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="38"/>
     </row>
@@ -1157,17 +1152,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="10"/>
     </row>
@@ -1176,17 +1171,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="10"/>
     </row>
@@ -1195,17 +1190,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I17" s="10"/>
     </row>
@@ -1214,14 +1209,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="10"/>

</xml_diff>